<commit_message>
Updated grading table for webterv
</commit_message>
<xml_diff>
--- a/teaching/webterv/webterv_merfoldko_01.xlsx
+++ b/teaching/webterv/webterv_merfoldko_01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumentumok\egyetem\oktatas\webterv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumentumok\egyetem\website\cservZ.github.io\teaching\webterv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A17FEA-3757-4A02-82F0-C07BA24FCEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE6C4DB-1486-4287-8910-61EBCE4E462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31CCB5CF-C965-4819-B7B9-D81D0E49B7CE}"/>
   </bookViews>
@@ -810,7 +810,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFCD442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -820,7 +820,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF99FF66"/>
+          <bgColor rgb="FF00CC5C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -850,7 +850,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF99FF66"/>
+          <bgColor rgb="FF00CC5C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -858,11 +858,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFCD442"/>
+      <color rgb="FFFBCD25"/>
+      <color rgb="FFFFCA21"/>
+      <color rgb="FF00CC5C"/>
+      <color rgb="FF00D25F"/>
+      <color rgb="FF00C85A"/>
+      <color rgb="FF4BE200"/>
       <color rgb="FF99FF66"/>
       <color rgb="FF00CC66"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FF00CC00"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1175,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A17724-C509-4255-B7CE-9CF8EDAA9016}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>

</xml_diff>